<commit_message>
Added a simple expected result check
</commit_message>
<xml_diff>
--- a/src/test/java/TestCases/SimpleCarJourney01.xlsx
+++ b/src/test/java/TestCases/SimpleCarJourney01.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="135">
   <si>
     <t>Element Type</t>
   </si>
@@ -254,9 +255,6 @@
     <t>first_name</t>
   </si>
   <si>
-    <t>Joe</t>
-  </si>
-  <si>
     <t>date_of_birth_dd</t>
   </si>
   <si>
@@ -328,9 +326,6 @@
     <t>surname</t>
   </si>
   <si>
-    <t>Smith</t>
-  </si>
-  <si>
     <t>//select[@name="title"]</t>
   </si>
   <si>
@@ -521,6 +516,24 @@
   </si>
   <si>
     <t>agreement</t>
+  </si>
+  <si>
+    <t>[Optional] Expected Result Operator</t>
+  </si>
+  <si>
+    <t>[Optional] Expected Result Value</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>contains</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we are currently searching </t>
+  </si>
+  <si>
+    <t>About you</t>
   </si>
 </sst>
 </file>
@@ -768,7 +781,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -797,6 +810,22 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -806,22 +835,9 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1103,21 +1119,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="28.296875" style="8" customWidth="1"/>
-    <col min="2" max="6" width="20.296875" style="9" customWidth="1"/>
+    <col min="2" max="8" width="20.296875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8" ht="26.4">
       <c r="A1" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -1132,10 +1148,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="31.2">
+    <row r="2" spans="1:8" ht="31.2">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1152,8 +1174,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -1170,8 +1194,10 @@
         <v>13</v>
       </c>
       <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
@@ -1182,16 +1208,18 @@
         <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
@@ -1202,16 +1230,18 @@
         <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" s="10" t="s">
         <v>32</v>
       </c>
@@ -1222,16 +1252,18 @@
         <v>32</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E6" s="4">
         <v>2015</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
@@ -1242,16 +1274,18 @@
         <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
@@ -1259,7 +1293,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>23</v>
@@ -1268,8 +1302,10 @@
         <v>4003</v>
       </c>
       <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="46.8">
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="46.8">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1286,8 +1322,10 @@
         <v>13</v>
       </c>
       <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="46.8">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="46.8">
       <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
@@ -1304,8 +1342,10 @@
         <v>13</v>
       </c>
       <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="46.8">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="46.8">
       <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
@@ -1322,8 +1362,10 @@
         <v>13</v>
       </c>
       <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="31.2">
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="31.2">
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
@@ -1334,14 +1376,16 @@
         <v>28</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" ht="62.4">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="62.4">
       <c r="A13" s="7" t="s">
         <v>30</v>
       </c>
@@ -1358,8 +1402,10 @@
         <v>13</v>
       </c>
       <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
@@ -1370,14 +1416,16 @@
         <v>31</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E14" s="4">
         <v>5</v>
       </c>
       <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
@@ -1393,27 +1441,37 @@
       <c r="E15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" ht="31.95" customHeight="1">
+      <c r="F15" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="31.95" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="C16" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" ht="31.95" customHeight="1">
+      <c r="C16" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="1:8" ht="31.95" customHeight="1">
       <c r="A17" s="7"/>
       <c r="C17" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" spans="1:6" ht="31.2">
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" ht="31.2">
       <c r="A18" s="7" t="s">
         <v>40</v>
       </c>
@@ -1421,19 +1479,21 @@
         <v>25</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:8">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
@@ -1447,91 +1507,101 @@
         <v>7</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>44</v>
+        <v>131</v>
       </c>
       <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="7" t="s">
+      <c r="B22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="7" t="s">
+      <c r="B23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>12</v>
@@ -1540,90 +1610,100 @@
         <v>13</v>
       </c>
       <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" ht="16.2">
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="16.2">
       <c r="A25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F25" s="4" t="s">
+    </row>
+    <row r="26" spans="1:8" ht="16.2">
+      <c r="A26" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="16.2">
-      <c r="A26" s="7" t="s">
+      <c r="B26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" ht="31.2">
+      <c r="A27" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:6" ht="31.2">
-      <c r="A27" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="B27" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" ht="16.2">
+      <c r="A28" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="1:6" ht="16.2">
-      <c r="A28" s="7" t="s">
-        <v>61</v>
-      </c>
       <c r="B28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="1:6" ht="16.2">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" ht="16.2">
       <c r="A29" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>12</v>
@@ -1632,16 +1712,18 @@
         <v>13</v>
       </c>
       <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="1:6" ht="46.8">
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" ht="46.8">
       <c r="A30" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>12</v>
@@ -1650,86 +1732,96 @@
         <v>13</v>
       </c>
       <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" ht="16.2">
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" ht="16.2">
       <c r="A31" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="19" t="s">
-        <v>82</v>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="19" t="s">
-        <v>82</v>
+      <c r="C32" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="31.2">
+      <c r="A33" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" ht="31.2">
-      <c r="A33" s="7" t="s">
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="4" t="s">
+    </row>
+    <row r="34" spans="1:8" ht="16.2">
+      <c r="A34" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="B34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="16.2">
-      <c r="A34" s="7" t="s">
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="7" t="s">
         <v>38</v>
       </c>
@@ -1746,131 +1838,147 @@
         <v>13</v>
       </c>
       <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="1:6" ht="31.95" customHeight="1">
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" ht="31.95" customHeight="1">
       <c r="A36" s="7"/>
       <c r="C36" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
-      <c r="F36" s="17"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="19" t="s">
-        <v>97</v>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="17"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="13" t="s">
+        <v>95</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="19" t="s">
-        <v>97</v>
+      <c r="C37" s="13" t="s">
+        <v>95</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E37" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="B38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="7" t="s">
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="4" t="s">
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="B39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="7" t="s">
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" ht="31.2">
+      <c r="A40" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" ht="31.2">
-      <c r="A40" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" s="4" t="s">
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F41" s="4"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="7" t="s">
         <v>38</v>
       </c>
@@ -1887,191 +1995,203 @@
         <v>13</v>
       </c>
       <c r="F43" s="4"/>
-    </row>
-    <row r="44" spans="1:6" ht="31.95" customHeight="1">
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" ht="31.95" customHeight="1">
       <c r="A44" s="7"/>
       <c r="C44" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
-      <c r="F44" s="17"/>
-    </row>
-    <row r="45" spans="1:6" ht="16.2">
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="17"/>
+    </row>
+    <row r="45" spans="1:8" ht="16.2">
       <c r="A45" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" ht="46.8">
+      <c r="A46" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="20" t="s">
+      <c r="B46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E45" s="4" t="s">
+      <c r="D46" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F45" s="4"/>
-    </row>
-    <row r="46" spans="1:6" ht="46.8">
-      <c r="A46" s="7" t="s">
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E46" s="4" t="s">
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F46" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="B47" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="19" t="s">
-        <v>109</v>
+      <c r="C47" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E47" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F47" s="4"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="7" t="s">
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="19" t="s">
+      <c r="B49" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E48" s="4" t="s">
+      <c r="D49" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E49" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F48" s="4"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="9" t="s">
+      <c r="H49" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E49" s="9" t="s">
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="B50" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H50" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="19" t="s">
+    <row r="51" spans="1:8">
+      <c r="A51" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="19" t="s">
+      <c r="B51" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F50" s="9" t="s">
+      <c r="D51" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="9" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="9" t="s">
+      <c r="B52" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B51" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="19" t="s">
+      <c r="B53" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="9" t="s">
+      <c r="D53" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H53" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B52" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="7" t="s">
         <v>38</v>
       </c>
@@ -2088,77 +2208,81 @@
         <v>13</v>
       </c>
       <c r="F54" s="4"/>
-    </row>
-    <row r="55" spans="1:6" ht="31.95" customHeight="1">
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:8" ht="31.95" customHeight="1">
       <c r="A55" s="7"/>
       <c r="C55" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
-      <c r="F55" s="17"/>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="17"/>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="19" t="s">
-        <v>122</v>
+      <c r="C56" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+        <v>121</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="19" t="s">
-        <v>128</v>
+      <c r="C57" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E57" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="B58" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H58" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F58" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:8">
       <c r="A59" s="7" t="s">
         <v>38</v>
       </c>
@@ -2175,25 +2299,29 @@
         <v>13</v>
       </c>
       <c r="F59" s="4"/>
-    </row>
-    <row r="60" spans="1:6" ht="31.95" customHeight="1">
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" spans="1:8" ht="31.95" customHeight="1">
       <c r="A60" s="7"/>
       <c r="C60" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
-      <c r="F60" s="17"/>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="19" t="s">
-        <v>130</v>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="17"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="13" t="s">
+        <v>128</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C61" s="19" t="s">
-        <v>130</v>
+      <c r="C61" s="13" t="s">
+        <v>128</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>12</v>
@@ -2202,7 +2330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:8" ht="31.2">
       <c r="A62" s="7" t="s">
         <v>38</v>
       </c>
@@ -2218,12 +2346,18 @@
       <c r="E62" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F62" s="4"/>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="F62" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="9"/>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:8">
       <c r="A64" s="9"/>
     </row>
     <row r="65" spans="1:1">
@@ -2246,12 +2380,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="C55:F55"/>
+    <mergeCell ref="C60:H60"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="C44:H44"/>
+    <mergeCell ref="C55:H55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E32" r:id="rId1"/>
@@ -2259,4 +2393,43 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.2">
+      <c r="A1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>